<commit_message>
flow control (if, elseif) added
added command for file execution and control structures
</commit_message>
<xml_diff>
--- a/WordList.xlsx
+++ b/WordList.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="113">
   <si>
     <t>Name</t>
   </si>
@@ -314,12 +314,6 @@
     <t>concat, length, etc…</t>
   </si>
   <si>
-    <t>control structures</t>
-  </si>
-  <si>
-    <t>if, else, elseif</t>
-  </si>
-  <si>
     <t>repeat, while, for, etc…</t>
   </si>
   <si>
@@ -333,6 +327,42 @@
   </si>
   <si>
     <t>Features to add</t>
+  </si>
+  <si>
+    <t>Flow Control</t>
+  </si>
+  <si>
+    <t>if</t>
+  </si>
+  <si>
+    <t>Bool, WordSet</t>
+  </si>
+  <si>
+    <t>Executes the Wordset if Bool on the stack is true.</t>
+  </si>
+  <si>
+    <t>ifelse</t>
+  </si>
+  <si>
+    <t>Bool, WordSet, WordSet</t>
+  </si>
+  <si>
+    <t>Executes the first WordSet if the Bool on the stack is true, the seconds, if the Bool is false.</t>
+  </si>
+  <si>
+    <t>exec</t>
+  </si>
+  <si>
+    <t>Files</t>
+  </si>
+  <si>
+    <t>Executes the file, specified by the String.</t>
+  </si>
+  <si>
+    <t>ccon</t>
+  </si>
+  <si>
+    <t>Clears the console.</t>
   </si>
 </sst>
 </file>
@@ -550,8 +580,77 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="dotted">
         <color indexed="64"/>
       </top>
       <bottom/>
@@ -561,12 +660,10 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="dotted">
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="dotted">
         <color indexed="64"/>
       </bottom>
@@ -580,7 +677,7 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="dotted">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -589,51 +686,10 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="dotted">
-        <color indexed="64"/>
-      </top>
-      <bottom style="dotted">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
+      <right style="dotted">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="dotted">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="dotted">
-        <color indexed="64"/>
-      </top>
-      <bottom style="dotted">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="dotted">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -644,33 +700,9 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="dotted">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="dotted">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -678,7 +710,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -703,29 +735,29 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -747,15 +779,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -763,132 +795,158 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1175,10 +1233,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:K32"/>
+  <dimension ref="B1:K46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1186,7 +1244,7 @@
     <col min="1" max="1" width="2.42578125" customWidth="1"/>
     <col min="2" max="2" width="22.42578125" customWidth="1"/>
     <col min="3" max="3" width="17.7109375" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" customWidth="1"/>
+    <col min="4" max="4" width="24" customWidth="1"/>
     <col min="5" max="5" width="19.140625" customWidth="1"/>
     <col min="6" max="6" width="33.5703125" customWidth="1"/>
     <col min="7" max="7" width="39.42578125" customWidth="1"/>
@@ -1218,34 +1276,34 @@
       <c r="E4" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="61" t="s">
+      <c r="F4" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="62"/>
+      <c r="G4" s="51"/>
       <c r="J4" s="40" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="K4" s="5" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="63" t="s">
+      <c r="B5" s="93" t="s">
         <v>92</v>
       </c>
-      <c r="C5" s="64" t="s">
+      <c r="C5" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="65" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="66" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="67" t="s">
+      <c r="D5" s="80" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="81" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="82" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="68"/>
+      <c r="G5" s="83"/>
       <c r="J5" s="42" t="s">
         <v>94</v>
       </c>
@@ -1254,155 +1312,149 @@
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="69"/>
-      <c r="C6" s="70" t="s">
+      <c r="B6" s="65"/>
+      <c r="C6" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="71" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="72" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="73" t="s">
+      <c r="D6" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="74"/>
-      <c r="J6" s="22" t="s">
-        <v>96</v>
-      </c>
-      <c r="K6" s="12" t="s">
-        <v>97</v>
-      </c>
+      <c r="G6" s="85"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="12"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="69"/>
-      <c r="C7" s="70" t="s">
+      <c r="B7" s="65"/>
+      <c r="C7" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="71" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="72" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="75" t="s">
+      <c r="D7" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="76"/>
+      <c r="G7" s="86"/>
       <c r="J7" s="22" t="s">
         <v>67</v>
       </c>
       <c r="K7" s="12" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="45" t="s">
+      <c r="B8" s="66"/>
+      <c r="C8" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="G8" s="86"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="12"/>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B9" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C9" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="24" t="s">
+      <c r="D9" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="25" t="s">
+      <c r="E9" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="25" t="s">
         <v>15</v>
-      </c>
-      <c r="G8" s="30"/>
-      <c r="J8" s="22" t="s">
-        <v>99</v>
-      </c>
-      <c r="K8" s="12"/>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="46"/>
-      <c r="C9" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="25" t="s">
-        <v>13</v>
       </c>
       <c r="G9" s="30"/>
       <c r="J9" s="22" t="s">
-        <v>100</v>
-      </c>
-      <c r="K9" s="12" t="s">
-        <v>101</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="K9" s="12"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="46"/>
+      <c r="B10" s="55"/>
       <c r="C10" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="30"/>
+      <c r="J10" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="K10" s="12" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="55"/>
+      <c r="C11" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="25" t="s">
+      <c r="D11" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="25" t="s">
         <v>14</v>
-      </c>
-      <c r="G10" s="30"/>
-      <c r="J10" s="22"/>
-      <c r="K10" s="12"/>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="47"/>
-      <c r="C11" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="D11" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="25" t="s">
-        <v>42</v>
       </c>
       <c r="G11" s="30"/>
       <c r="J11" s="22"/>
       <c r="K11" s="12"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="59" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="E12" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="F12" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="G12" s="18" t="s">
-        <v>27</v>
-      </c>
+      <c r="B12" s="56"/>
+      <c r="C12" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" s="30"/>
       <c r="J12" s="22"/>
       <c r="K12" s="12"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="60"/>
+      <c r="B13" s="69" t="s">
+        <v>24</v>
+      </c>
       <c r="C13" s="16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D13" s="17" t="s">
         <v>86</v>
@@ -1411,18 +1463,18 @@
         <v>26</v>
       </c>
       <c r="F13" s="31" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G13" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J13" s="22"/>
       <c r="K13" s="12"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="60"/>
+      <c r="B14" s="70"/>
       <c r="C14" s="16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D14" s="17" t="s">
         <v>86</v>
@@ -1431,18 +1483,18 @@
         <v>26</v>
       </c>
       <c r="F14" s="31" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G14" s="18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J14" s="22"/>
       <c r="K14" s="12"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="60"/>
+      <c r="B15" s="70"/>
       <c r="C15" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D15" s="17" t="s">
         <v>86</v>
@@ -1451,18 +1503,18 @@
         <v>26</v>
       </c>
       <c r="F15" s="31" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G15" s="18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J15" s="22"/>
       <c r="K15" s="12"/>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="60"/>
+      <c r="B16" s="70"/>
       <c r="C16" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D16" s="17" t="s">
         <v>86</v>
@@ -1471,310 +1523,312 @@
         <v>26</v>
       </c>
       <c r="F16" s="31" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G16" s="18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J16" s="22"/>
       <c r="K16" s="12"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="77" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" s="70" t="s">
-        <v>38</v>
-      </c>
-      <c r="D17" s="71" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" s="72" t="s">
-        <v>10</v>
-      </c>
-      <c r="F17" s="75" t="s">
-        <v>39</v>
-      </c>
-      <c r="G17" s="72"/>
+      <c r="B17" s="70"/>
+      <c r="C17" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="G17" s="18" t="s">
+        <v>31</v>
+      </c>
       <c r="J17" s="22"/>
       <c r="K17" s="12"/>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="80"/>
-      <c r="C18" s="70" t="s">
-        <v>93</v>
-      </c>
-      <c r="D18" s="71" t="s">
-        <v>10</v>
-      </c>
-      <c r="E18" s="72" t="s">
-        <v>10</v>
-      </c>
-      <c r="F18" s="81" t="s">
-        <v>40</v>
-      </c>
-      <c r="G18" s="72"/>
+      <c r="B18" s="52" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="45" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="48" t="s">
+        <v>39</v>
+      </c>
+      <c r="G18" s="47"/>
       <c r="J18" s="22"/>
       <c r="K18" s="12"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="50" t="s">
-        <v>48</v>
-      </c>
-      <c r="C19" s="32" t="s">
-        <v>45</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F19" s="33" t="s">
-        <v>57</v>
-      </c>
-      <c r="G19" s="13"/>
+      <c r="B19" s="57"/>
+      <c r="C19" s="45" t="s">
+        <v>93</v>
+      </c>
+      <c r="D19" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="49" t="s">
+        <v>40</v>
+      </c>
+      <c r="G19" s="47"/>
       <c r="J19" s="22"/>
       <c r="K19" s="12"/>
     </row>
-    <row r="20" spans="2:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="51"/>
-      <c r="C20" s="34" t="s">
-        <v>43</v>
-      </c>
-      <c r="D20" s="35" t="s">
-        <v>44</v>
-      </c>
-      <c r="E20" s="36" t="s">
-        <v>10</v>
-      </c>
-      <c r="F20" s="48" t="s">
-        <v>47</v>
-      </c>
-      <c r="G20" s="49"/>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B20" s="60" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F20" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="G20" s="13"/>
       <c r="J20" s="22"/>
       <c r="K20" s="12"/>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B21" s="52" t="s">
-        <v>53</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E21" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="F21" s="29" t="s">
-        <v>55</v>
-      </c>
-      <c r="G21" s="14"/>
+    <row r="21" spans="2:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="61"/>
+      <c r="C21" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" s="58" t="s">
+        <v>47</v>
+      </c>
+      <c r="G21" s="59"/>
       <c r="J21" s="22"/>
       <c r="K21" s="12"/>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="53"/>
+      <c r="B22" s="62" t="s">
+        <v>53</v>
+      </c>
       <c r="C22" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>58</v>
+        <v>10</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F22" s="29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G22" s="14"/>
       <c r="J22" s="22"/>
       <c r="K22" s="12"/>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="54" t="s">
-        <v>59</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E23" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="F23" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="G23" s="15"/>
+      <c r="B23" s="63"/>
+      <c r="C23" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F23" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="G23" s="14"/>
       <c r="J23" s="22"/>
       <c r="K23" s="12"/>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B24" s="55"/>
+      <c r="B24" s="64" t="s">
+        <v>59</v>
+      </c>
       <c r="C24" s="11" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>10</v>
       </c>
       <c r="E24" s="15" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G24" s="15"/>
       <c r="J24" s="22"/>
       <c r="K24" s="12"/>
     </row>
-    <row r="25" spans="2:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="56"/>
-      <c r="C25" s="38" t="s">
-        <v>62</v>
-      </c>
-      <c r="D25" s="37" t="s">
-        <v>10</v>
-      </c>
-      <c r="E25" s="39" t="s">
-        <v>63</v>
-      </c>
-      <c r="F25" s="57" t="s">
-        <v>66</v>
-      </c>
-      <c r="G25" s="58"/>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B25" s="65"/>
+      <c r="C25" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="G25" s="15"/>
       <c r="J25" s="22"/>
       <c r="K25" s="12"/>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B26" s="77" t="s">
-        <v>79</v>
-      </c>
-      <c r="C26" s="70" t="s">
-        <v>71</v>
-      </c>
-      <c r="D26" s="70" t="s">
-        <v>26</v>
-      </c>
-      <c r="E26" s="70" t="s">
-        <v>26</v>
-      </c>
-      <c r="F26" s="78" t="s">
-        <v>78</v>
-      </c>
-      <c r="G26" s="72" t="s">
-        <v>84</v>
-      </c>
+    <row r="26" spans="2:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="66"/>
+      <c r="C26" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="D26" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="F26" s="67" t="s">
+        <v>66</v>
+      </c>
+      <c r="G26" s="68"/>
       <c r="J26" s="22"/>
       <c r="K26" s="12"/>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B27" s="79"/>
-      <c r="C27" s="70" t="s">
-        <v>68</v>
-      </c>
-      <c r="D27" s="71" t="s">
-        <v>86</v>
-      </c>
-      <c r="E27" s="72" t="s">
-        <v>61</v>
-      </c>
-      <c r="F27" s="75" t="s">
-        <v>77</v>
-      </c>
-      <c r="G27" s="72" t="s">
-        <v>74</v>
+      <c r="B27" s="52" t="s">
+        <v>79</v>
+      </c>
+      <c r="C27" s="45" t="s">
+        <v>71</v>
+      </c>
+      <c r="D27" s="45" t="s">
+        <v>26</v>
+      </c>
+      <c r="E27" s="45" t="s">
+        <v>26</v>
+      </c>
+      <c r="F27" s="91" t="s">
+        <v>78</v>
+      </c>
+      <c r="G27" s="92" t="s">
+        <v>84</v>
       </c>
       <c r="J27" s="22"/>
       <c r="K27" s="12"/>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B28" s="79"/>
-      <c r="C28" s="70" t="s">
-        <v>69</v>
-      </c>
-      <c r="D28" s="71" t="s">
+      <c r="B28" s="53"/>
+      <c r="C28" s="45" t="s">
+        <v>68</v>
+      </c>
+      <c r="D28" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="E28" s="72" t="s">
+      <c r="E28" s="47" t="s">
         <v>61</v>
       </c>
-      <c r="F28" s="75" t="s">
-        <v>72</v>
-      </c>
-      <c r="G28" s="72" t="s">
-        <v>75</v>
+      <c r="F28" s="48" t="s">
+        <v>77</v>
+      </c>
+      <c r="G28" s="47" t="s">
+        <v>74</v>
       </c>
       <c r="J28" s="22"/>
       <c r="K28" s="12"/>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B29" s="79"/>
-      <c r="C29" s="70" t="s">
-        <v>70</v>
-      </c>
-      <c r="D29" s="71" t="s">
+      <c r="B29" s="53"/>
+      <c r="C29" s="45" t="s">
+        <v>69</v>
+      </c>
+      <c r="D29" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="E29" s="72" t="s">
+      <c r="E29" s="47" t="s">
         <v>61</v>
       </c>
-      <c r="F29" s="75" t="s">
-        <v>73</v>
-      </c>
-      <c r="G29" s="72" t="s">
-        <v>76</v>
+      <c r="F29" s="48" t="s">
+        <v>72</v>
+      </c>
+      <c r="G29" s="47" t="s">
+        <v>75</v>
       </c>
       <c r="J29" s="22"/>
       <c r="K29" s="12"/>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B30" s="45" t="s">
-        <v>80</v>
-      </c>
-      <c r="C30" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="D30" s="4" t="s">
+      <c r="B30" s="53"/>
+      <c r="C30" s="45" t="s">
+        <v>70</v>
+      </c>
+      <c r="D30" s="46" t="s">
+        <v>86</v>
+      </c>
+      <c r="E30" s="47" t="s">
         <v>61</v>
       </c>
-      <c r="E30" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F30" s="43" t="s">
-        <v>88</v>
-      </c>
-      <c r="G30" s="44" t="s">
-        <v>89</v>
+      <c r="F30" s="48" t="s">
+        <v>73</v>
+      </c>
+      <c r="G30" s="47" t="s">
+        <v>76</v>
       </c>
       <c r="J30" s="22"/>
       <c r="K30" s="12"/>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B31" s="46"/>
-      <c r="C31" s="27" t="s">
-        <v>82</v>
-      </c>
-      <c r="D31" s="24" t="s">
-        <v>87</v>
-      </c>
-      <c r="E31" s="26" t="s">
+      <c r="B31" s="54" t="s">
+        <v>80</v>
+      </c>
+      <c r="C31" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="D31" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F31" s="28"/>
-      <c r="G31" s="26" t="s">
-        <v>90</v>
+      <c r="E31" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F31" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="G31" s="44" t="s">
+        <v>89</v>
       </c>
       <c r="J31" s="22"/>
       <c r="K31" s="12"/>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B32" s="47"/>
+      <c r="B32" s="55"/>
       <c r="C32" s="27" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D32" s="24" t="s">
         <v>87</v>
@@ -1784,25 +1838,177 @@
       </c>
       <c r="F32" s="28"/>
       <c r="G32" s="26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J32" s="22"/>
       <c r="K32" s="12"/>
     </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B33" s="56"/>
+      <c r="C33" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="D33" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="E33" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="F33" s="28"/>
+      <c r="G33" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="J33" s="22"/>
+      <c r="K33" s="12"/>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B34" s="73" t="s">
+        <v>101</v>
+      </c>
+      <c r="C34" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="D34" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="E34" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F34" s="71" t="s">
+        <v>104</v>
+      </c>
+      <c r="G34" s="74"/>
+    </row>
+    <row r="35" spans="2:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="73"/>
+      <c r="C35" s="76" t="s">
+        <v>105</v>
+      </c>
+      <c r="D35" s="77" t="s">
+        <v>106</v>
+      </c>
+      <c r="E35" s="78" t="s">
+        <v>10</v>
+      </c>
+      <c r="F35" s="72" t="s">
+        <v>107</v>
+      </c>
+      <c r="G35" s="75"/>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B36" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F36" s="87" t="s">
+        <v>110</v>
+      </c>
+      <c r="G36" s="88"/>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B37" s="89"/>
+      <c r="C37" s="89"/>
+      <c r="D37" s="89"/>
+      <c r="E37" s="89"/>
+      <c r="F37" s="90"/>
+      <c r="G37" s="12"/>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B38" s="89"/>
+      <c r="C38" s="89"/>
+      <c r="D38" s="89"/>
+      <c r="E38" s="89"/>
+      <c r="F38" s="90"/>
+      <c r="G38" s="12"/>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B39" s="89"/>
+      <c r="C39" s="89"/>
+      <c r="D39" s="89"/>
+      <c r="E39" s="89"/>
+      <c r="F39" s="90"/>
+      <c r="G39" s="12"/>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B40" s="89"/>
+      <c r="C40" s="89"/>
+      <c r="D40" s="89"/>
+      <c r="E40" s="89"/>
+      <c r="F40" s="90"/>
+      <c r="G40" s="12"/>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B41" s="89"/>
+      <c r="C41" s="89"/>
+      <c r="D41" s="89"/>
+      <c r="E41" s="89"/>
+      <c r="F41" s="90"/>
+      <c r="G41" s="12"/>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B42" s="89"/>
+      <c r="C42" s="89"/>
+      <c r="D42" s="89"/>
+      <c r="E42" s="89"/>
+      <c r="F42" s="90"/>
+      <c r="G42" s="12"/>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B43" s="89"/>
+      <c r="C43" s="89"/>
+      <c r="D43" s="89"/>
+      <c r="E43" s="89"/>
+      <c r="F43" s="90"/>
+      <c r="G43" s="12"/>
+    </row>
+    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B44" s="89"/>
+      <c r="C44" s="89"/>
+      <c r="D44" s="89"/>
+      <c r="E44" s="89"/>
+      <c r="F44" s="90"/>
+      <c r="G44" s="12"/>
+    </row>
+    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B45" s="89"/>
+      <c r="C45" s="89"/>
+      <c r="D45" s="89"/>
+      <c r="E45" s="89"/>
+      <c r="F45" s="90"/>
+      <c r="G45" s="12"/>
+    </row>
+    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B46" s="89"/>
+      <c r="C46" s="89"/>
+      <c r="D46" s="89"/>
+      <c r="E46" s="89"/>
+      <c r="F46" s="90"/>
+      <c r="G46" s="12"/>
+    </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="B5:B7"/>
+  <mergeCells count="14">
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="B5:B8"/>
     <mergeCell ref="F4:G4"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="B30:B32"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="B12:B16"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="B13:B17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
loops, loops, loops, ...
fixed regex to accommodate tabs
added while loop
added conversion to string and bool
added getchar command for processing strings
added straightforward implementation of fletcher checksum
</commit_message>
<xml_diff>
--- a/WordList.xlsx
+++ b/WordList.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="147">
   <si>
     <t>Name</t>
   </si>
@@ -59,9 +59,6 @@
     <t>-</t>
   </si>
   <si>
-    <t>top</t>
-  </si>
-  <si>
     <t>Resets the interpreter. Clears stack, dictionary.</t>
   </si>
   <si>
@@ -423,6 +420,51 @@
   </si>
   <si>
     <t>Conversion</t>
+  </si>
+  <si>
+    <t>tostr</t>
+  </si>
+  <si>
+    <t>Int|Bool</t>
+  </si>
+  <si>
+    <t>Converts an Int or Bool to a String.</t>
+  </si>
+  <si>
+    <t>tobool</t>
+  </si>
+  <si>
+    <t>Converts an Int to a Bool. Result is true if integer is non-zero.</t>
+  </si>
+  <si>
+    <t>while</t>
+  </si>
+  <si>
+    <t>logical and</t>
+  </si>
+  <si>
+    <t>logical or</t>
+  </si>
+  <si>
+    <t>Executes a Wordset as long as Bool on top of stack is true.</t>
+  </si>
+  <si>
+    <t>getchar</t>
+  </si>
+  <si>
+    <t>String, Int</t>
+  </si>
+  <si>
+    <t>Pushes the value of the character at the specified index of the string to the stack.</t>
+  </si>
+  <si>
+    <t>object</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>Prints integer in hex format (base 16).</t>
   </si>
 </sst>
 </file>
@@ -770,7 +812,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -931,81 +973,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1024,8 +991,93 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1313,10 +1365,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:K47"/>
+  <dimension ref="B1:K50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1334,18 +1386,18 @@
   <sheetData>
     <row r="1" spans="2:11" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B1" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C4" s="20" t="s">
         <v>0</v>
@@ -1356,20 +1408,20 @@
       <c r="E4" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="74" t="s">
+      <c r="F4" s="88" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="75"/>
+      <c r="G4" s="89"/>
       <c r="J4" s="40" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K4" s="5" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="71" t="s">
-        <v>92</v>
+      <c r="B5" s="87" t="s">
+        <v>91</v>
       </c>
       <c r="C5" s="55" t="s">
         <v>4</v>
@@ -1381,18 +1433,18 @@
         <v>10</v>
       </c>
       <c r="F5" s="58" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G5" s="59"/>
       <c r="J5" s="42" t="s">
+        <v>93</v>
+      </c>
+      <c r="K5" s="41" t="s">
         <v>94</v>
       </c>
-      <c r="K5" s="41" t="s">
-        <v>95</v>
-      </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="72"/>
+      <c r="B6" s="79"/>
       <c r="C6" s="11" t="s">
         <v>8</v>
       </c>
@@ -1403,14 +1455,14 @@
         <v>10</v>
       </c>
       <c r="F6" s="60" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G6" s="61"/>
       <c r="J6" s="22"/>
       <c r="K6" s="12"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="72"/>
+      <c r="B7" s="79"/>
       <c r="C7" s="11" t="s">
         <v>9</v>
       </c>
@@ -1421,240 +1473,240 @@
         <v>10</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G7" s="62"/>
       <c r="J7" s="22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K7" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="73"/>
+      <c r="B8" s="80"/>
       <c r="C8" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="9" t="s">
         <v>111</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>112</v>
       </c>
       <c r="G8" s="62"/>
       <c r="J8" s="22"/>
       <c r="K8" s="12"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="78" t="s">
-        <v>25</v>
+      <c r="B9" s="92" t="s">
+        <v>24</v>
       </c>
       <c r="C9" s="27" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>11</v>
+        <v>144</v>
       </c>
       <c r="E9" s="26" t="s">
         <v>10</v>
       </c>
       <c r="F9" s="25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G9" s="30"/>
       <c r="J9" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="K9" s="12"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B10" s="93"/>
+      <c r="C10" s="27" t="s">
+        <v>145</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="G10" s="30"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="12"/>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="93"/>
+      <c r="C11" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="30"/>
+      <c r="J11" s="22" t="s">
         <v>97</v>
       </c>
-      <c r="K9" s="12"/>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="79"/>
-      <c r="C10" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="25" t="s">
+      <c r="K11" s="12" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="93"/>
+      <c r="C12" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="25" t="s">
         <v>13</v>
-      </c>
-      <c r="G10" s="30"/>
-      <c r="J10" s="22" t="s">
-        <v>98</v>
-      </c>
-      <c r="K10" s="12" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="79"/>
-      <c r="C11" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="G11" s="30"/>
-      <c r="J11" s="22"/>
-      <c r="K11" s="12"/>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="80"/>
-      <c r="C12" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="25" t="s">
-        <v>42</v>
       </c>
       <c r="G12" s="30"/>
       <c r="J12" s="22"/>
       <c r="K12" s="12"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="91" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="E13" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="F13" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="G13" s="18" t="s">
-        <v>27</v>
-      </c>
+      <c r="B13" s="94"/>
+      <c r="C13" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="G13" s="30"/>
       <c r="J13" s="22"/>
       <c r="K13" s="12"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="92"/>
+      <c r="B14" s="102" t="s">
+        <v>23</v>
+      </c>
       <c r="C14" s="16" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F14" s="31" t="s">
         <v>35</v>
       </c>
       <c r="G14" s="18" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="J14" s="22"/>
       <c r="K14" s="12"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="92"/>
+      <c r="B15" s="103"/>
       <c r="C15" s="16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F15" s="31" t="s">
         <v>34</v>
       </c>
       <c r="G15" s="18" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J15" s="22"/>
       <c r="K15" s="12"/>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="92"/>
+      <c r="B16" s="103"/>
       <c r="C16" s="16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F16" s="31" t="s">
         <v>33</v>
       </c>
       <c r="G16" s="18" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J16" s="22"/>
       <c r="K16" s="12"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="92"/>
+      <c r="B17" s="103"/>
       <c r="C17" s="16" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F17" s="31" t="s">
         <v>32</v>
       </c>
       <c r="G17" s="18" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J17" s="22"/>
       <c r="K17" s="12"/>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="76" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" s="45" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" s="46" t="s">
-        <v>10</v>
-      </c>
-      <c r="E18" s="47" t="s">
-        <v>10</v>
-      </c>
-      <c r="F18" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="G18" s="47"/>
+      <c r="B18" s="103"/>
+      <c r="C18" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F18" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="G18" s="18" t="s">
+        <v>30</v>
+      </c>
       <c r="J18" s="22"/>
       <c r="K18" s="12"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="81"/>
+      <c r="B19" s="90" t="s">
+        <v>36</v>
+      </c>
       <c r="C19" s="45" t="s">
-        <v>93</v>
+        <v>37</v>
       </c>
       <c r="D19" s="46" t="s">
         <v>10</v>
@@ -1662,508 +1714,581 @@
       <c r="E19" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="F19" s="49" t="s">
-        <v>40</v>
+      <c r="F19" s="48" t="s">
+        <v>38</v>
       </c>
       <c r="G19" s="47"/>
       <c r="J19" s="22"/>
       <c r="K19" s="12"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="84" t="s">
-        <v>48</v>
-      </c>
-      <c r="C20" s="32" t="s">
-        <v>45</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F20" s="33" t="s">
-        <v>57</v>
-      </c>
-      <c r="G20" s="13"/>
+      <c r="B20" s="95"/>
+      <c r="C20" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="D20" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" s="49" t="s">
+        <v>39</v>
+      </c>
+      <c r="G20" s="47"/>
       <c r="J20" s="22"/>
       <c r="K20" s="12"/>
     </row>
-    <row r="21" spans="2:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="103"/>
-      <c r="C21" s="34" t="s">
-        <v>43</v>
-      </c>
-      <c r="D21" s="35" t="s">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B21" s="81" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="E21" s="36" t="s">
-        <v>10</v>
-      </c>
-      <c r="F21" s="82" t="s">
-        <v>47</v>
-      </c>
-      <c r="G21" s="83"/>
+      <c r="D21" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F21" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="G21" s="13"/>
       <c r="J21" s="22"/>
       <c r="K21" s="12"/>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="85"/>
+    <row r="22" spans="2:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="82"/>
       <c r="C22" s="34" t="s">
-        <v>130</v>
+        <v>42</v>
       </c>
       <c r="D22" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" s="96" t="s">
         <v>46</v>
       </c>
-      <c r="E22" s="36" t="s">
-        <v>10</v>
-      </c>
-      <c r="F22" s="101" t="s">
-        <v>131</v>
-      </c>
-      <c r="G22" s="102"/>
+      <c r="G22" s="97"/>
       <c r="J22" s="22"/>
       <c r="K22" s="12"/>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="86" t="s">
-        <v>53</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E23" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="F23" s="29" t="s">
-        <v>55</v>
-      </c>
-      <c r="G23" s="14"/>
+      <c r="B23" s="83"/>
+      <c r="C23" s="34" t="s">
+        <v>129</v>
+      </c>
+      <c r="D23" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="E23" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" s="76" t="s">
+        <v>130</v>
+      </c>
+      <c r="G23" s="77"/>
       <c r="J23" s="22"/>
       <c r="K23" s="12"/>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B24" s="87"/>
+      <c r="B24" s="98" t="s">
+        <v>52</v>
+      </c>
       <c r="C24" s="10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>58</v>
+        <v>10</v>
       </c>
       <c r="E24" s="14" t="s">
         <v>53</v>
       </c>
       <c r="F24" s="29" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G24" s="14"/>
       <c r="J24" s="22"/>
       <c r="K24" s="12"/>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B25" s="88" t="s">
-        <v>59</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E25" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="F25" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="G25" s="15"/>
+      <c r="B25" s="99"/>
+      <c r="C25" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="F25" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="G25" s="14"/>
       <c r="J25" s="22"/>
       <c r="K25" s="12"/>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B26" s="72"/>
+      <c r="B26" s="78" t="s">
+        <v>58</v>
+      </c>
       <c r="C26" s="11" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="D26" s="8" t="s">
         <v>10</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>26</v>
+        <v>60</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G26" s="15"/>
       <c r="J26" s="22"/>
       <c r="K26" s="12"/>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B27" s="73"/>
-      <c r="C27" s="38" t="s">
-        <v>62</v>
-      </c>
-      <c r="D27" s="37" t="s">
-        <v>10</v>
-      </c>
-      <c r="E27" s="39" t="s">
-        <v>63</v>
-      </c>
-      <c r="F27" s="89" t="s">
-        <v>66</v>
-      </c>
-      <c r="G27" s="90"/>
+      <c r="B27" s="79"/>
+      <c r="C27" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="G27" s="15"/>
       <c r="J27" s="22"/>
       <c r="K27" s="12"/>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B28" s="76" t="s">
-        <v>79</v>
-      </c>
-      <c r="C28" s="45" t="s">
-        <v>71</v>
-      </c>
-      <c r="D28" s="45" t="s">
-        <v>26</v>
-      </c>
-      <c r="E28" s="45" t="s">
-        <v>26</v>
-      </c>
-      <c r="F28" s="66" t="s">
-        <v>78</v>
-      </c>
-      <c r="G28" s="67" t="s">
-        <v>84</v>
-      </c>
+      <c r="B28" s="80"/>
+      <c r="C28" s="38" t="s">
+        <v>61</v>
+      </c>
+      <c r="D28" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" s="39" t="s">
+        <v>62</v>
+      </c>
+      <c r="F28" s="100" t="s">
+        <v>65</v>
+      </c>
+      <c r="G28" s="101"/>
       <c r="J28" s="22"/>
       <c r="K28" s="12"/>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B29" s="77"/>
+      <c r="B29" s="90" t="s">
+        <v>78</v>
+      </c>
       <c r="C29" s="45" t="s">
-        <v>68</v>
-      </c>
-      <c r="D29" s="46" t="s">
-        <v>86</v>
-      </c>
-      <c r="E29" s="47" t="s">
-        <v>61</v>
-      </c>
-      <c r="F29" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D29" s="45" t="s">
+        <v>25</v>
+      </c>
+      <c r="E29" s="45" t="s">
+        <v>25</v>
+      </c>
+      <c r="F29" s="66" t="s">
         <v>77</v>
       </c>
-      <c r="G29" s="47" t="s">
-        <v>74</v>
+      <c r="G29" s="67" t="s">
+        <v>83</v>
       </c>
       <c r="J29" s="22"/>
       <c r="K29" s="12"/>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B30" s="77"/>
+      <c r="B30" s="91"/>
       <c r="C30" s="45" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D30" s="46" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E30" s="47" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F30" s="48" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="G30" s="47" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J30" s="22"/>
       <c r="K30" s="12"/>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B31" s="77"/>
+      <c r="B31" s="91"/>
       <c r="C31" s="45" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D31" s="46" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E31" s="47" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F31" s="48" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G31" s="47" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J31" s="22"/>
       <c r="K31" s="12"/>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B32" s="78" t="s">
-        <v>80</v>
-      </c>
-      <c r="C32" s="23" t="s">
+      <c r="B32" s="91"/>
+      <c r="C32" s="45" t="s">
+        <v>69</v>
+      </c>
+      <c r="D32" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="D32" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F32" s="43" t="s">
-        <v>88</v>
-      </c>
-      <c r="G32" s="44" t="s">
-        <v>89</v>
+      <c r="E32" s="47" t="s">
+        <v>60</v>
+      </c>
+      <c r="F32" s="48" t="s">
+        <v>72</v>
+      </c>
+      <c r="G32" s="47" t="s">
+        <v>75</v>
       </c>
       <c r="J32" s="22"/>
       <c r="K32" s="12"/>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B33" s="79"/>
-      <c r="C33" s="27" t="s">
-        <v>82</v>
-      </c>
-      <c r="D33" s="24" t="s">
+      <c r="B33" s="92" t="s">
+        <v>79</v>
+      </c>
+      <c r="C33" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F33" s="43" t="s">
         <v>87</v>
       </c>
-      <c r="E33" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="F33" s="28"/>
-      <c r="G33" s="26" t="s">
-        <v>90</v>
+      <c r="G33" s="44" t="s">
+        <v>88</v>
       </c>
       <c r="J33" s="22"/>
       <c r="K33" s="12"/>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B34" s="80"/>
+      <c r="B34" s="93"/>
       <c r="C34" s="27" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D34" s="24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E34" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="F34" s="28"/>
+        <v>60</v>
+      </c>
+      <c r="F34" s="28" t="s">
+        <v>138</v>
+      </c>
       <c r="G34" s="26" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J34" s="22"/>
       <c r="K34" s="12"/>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B35" s="70" t="s">
+      <c r="B35" s="94"/>
+      <c r="C35" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="D35" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="E35" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="F35" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="G35" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="J35" s="22"/>
+      <c r="K35" s="12"/>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B36" s="86" t="s">
+        <v>100</v>
+      </c>
+      <c r="C36" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="C35" s="16" t="s">
+      <c r="D36" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="D35" s="17" t="s">
+      <c r="E36" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F36" s="50" t="s">
         <v>103</v>
       </c>
-      <c r="E35" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="F35" s="50" t="s">
+      <c r="G36" s="51"/>
+    </row>
+    <row r="37" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="86"/>
+      <c r="C37" s="52" t="s">
         <v>104</v>
       </c>
-      <c r="G35" s="51"/>
-    </row>
-    <row r="36" spans="2:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="70"/>
-      <c r="C36" s="52" t="s">
+      <c r="D37" s="53" t="s">
         <v>105</v>
       </c>
-      <c r="D36" s="53" t="s">
+      <c r="E37" s="54" t="s">
+        <v>10</v>
+      </c>
+      <c r="F37" s="84" t="s">
         <v>106</v>
       </c>
-      <c r="E36" s="54" t="s">
-        <v>10</v>
-      </c>
-      <c r="F36" s="68" t="s">
+      <c r="G37" s="85"/>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B38" s="35" t="s">
+        <v>108</v>
+      </c>
+      <c r="C38" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="G36" s="69"/>
-    </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B37" s="35" t="s">
+      <c r="D38" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F38" s="63" t="s">
         <v>109</v>
       </c>
-      <c r="C37" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="D37" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="E37" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F37" s="63" t="s">
-        <v>110</v>
-      </c>
-      <c r="G37" s="64"/>
-    </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B38" s="93" t="s">
+      <c r="G38" s="64"/>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B39" s="68" t="s">
+        <v>112</v>
+      </c>
+      <c r="C39" s="68" t="s">
         <v>113</v>
       </c>
-      <c r="C38" s="93" t="s">
+      <c r="D39" s="68" t="s">
+        <v>10</v>
+      </c>
+      <c r="E39" s="68" t="s">
+        <v>62</v>
+      </c>
+      <c r="F39" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="D38" s="93" t="s">
-        <v>10</v>
-      </c>
-      <c r="E38" s="93" t="s">
-        <v>63</v>
-      </c>
-      <c r="F38" s="94" t="s">
+      <c r="G39" s="70"/>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B40" s="78" t="s">
         <v>115</v>
       </c>
-      <c r="G38" s="95"/>
-    </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B39" s="88" t="s">
+      <c r="C40" s="37" t="s">
         <v>116</v>
       </c>
-      <c r="C39" s="37" t="s">
+      <c r="D40" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="E40" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="F40" s="71" t="s">
+        <v>119</v>
+      </c>
+      <c r="G40" s="72"/>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B41" s="79"/>
+      <c r="C41" s="37" t="s">
         <v>117</v>
       </c>
-      <c r="D39" s="37" t="s">
-        <v>63</v>
-      </c>
-      <c r="E39" s="37" t="s">
-        <v>26</v>
-      </c>
-      <c r="F39" s="96" t="s">
+      <c r="D41" s="37" t="s">
+        <v>118</v>
+      </c>
+      <c r="E41" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="F41" s="71" t="s">
         <v>120</v>
       </c>
-      <c r="G39" s="97"/>
-    </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B40" s="72"/>
-      <c r="C40" s="37" t="s">
+      <c r="G41" s="72"/>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B42" s="79"/>
+      <c r="C42" s="37" t="s">
+        <v>121</v>
+      </c>
+      <c r="D42" s="37" t="s">
         <v>118</v>
       </c>
-      <c r="D40" s="37" t="s">
-        <v>119</v>
-      </c>
-      <c r="E40" s="37" t="s">
-        <v>63</v>
-      </c>
-      <c r="F40" s="96" t="s">
-        <v>121</v>
-      </c>
-      <c r="G40" s="97"/>
-    </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B41" s="72"/>
-      <c r="C41" s="37" t="s">
+      <c r="E42" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="F42" s="71" t="s">
         <v>122</v>
       </c>
-      <c r="D41" s="37" t="s">
-        <v>119</v>
-      </c>
-      <c r="E41" s="37" t="s">
-        <v>61</v>
-      </c>
-      <c r="F41" s="96" t="s">
+      <c r="G42" s="72"/>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B43" s="79"/>
+      <c r="C43" s="37" t="s">
         <v>123</v>
       </c>
-      <c r="G41" s="97"/>
-    </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B42" s="73"/>
-      <c r="C42" s="37" t="s">
+      <c r="D43" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="E43" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="F43" s="71" t="s">
         <v>124</v>
       </c>
-      <c r="D42" s="37" t="s">
-        <v>63</v>
-      </c>
-      <c r="E42" s="37" t="s">
-        <v>63</v>
-      </c>
-      <c r="F42" s="96" t="s">
+      <c r="G43" s="72"/>
+    </row>
+    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B44" s="80"/>
+      <c r="C44" s="37" t="s">
+        <v>141</v>
+      </c>
+      <c r="D44" s="37" t="s">
+        <v>142</v>
+      </c>
+      <c r="E44" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="F44" s="71" t="s">
+        <v>143</v>
+      </c>
+      <c r="G44" s="72"/>
+    </row>
+    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B45" s="90" t="s">
         <v>125</v>
       </c>
-      <c r="G42" s="97"/>
-    </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B43" s="98" t="s">
+      <c r="C45" s="73" t="s">
         <v>126</v>
       </c>
-      <c r="C43" s="98" t="s">
+      <c r="D45" s="73" t="s">
         <v>127</v>
       </c>
-      <c r="D43" s="98" t="s">
+      <c r="E45" s="73" t="s">
+        <v>10</v>
+      </c>
+      <c r="F45" s="74" t="s">
         <v>128</v>
       </c>
-      <c r="E43" s="98" t="s">
-        <v>10</v>
-      </c>
-      <c r="F43" s="99" t="s">
-        <v>129</v>
-      </c>
-      <c r="G43" s="100"/>
-    </row>
-    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B44" s="22" t="s">
+      <c r="G45" s="75"/>
+    </row>
+    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B46" s="95"/>
+      <c r="C46" s="73" t="s">
+        <v>137</v>
+      </c>
+      <c r="D46" s="73" t="s">
+        <v>102</v>
+      </c>
+      <c r="E46" s="73" t="s">
+        <v>10</v>
+      </c>
+      <c r="F46" s="106" t="s">
+        <v>140</v>
+      </c>
+      <c r="G46" s="107"/>
+    </row>
+    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B47" s="92" t="s">
+        <v>131</v>
+      </c>
+      <c r="C47" s="104" t="s">
         <v>132</v>
       </c>
-      <c r="C44" s="22"/>
-      <c r="D44" s="22"/>
-      <c r="E44" s="22"/>
-      <c r="F44" s="65"/>
-      <c r="G44" s="12"/>
-    </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B45" s="22"/>
-      <c r="C45" s="22"/>
-      <c r="D45" s="22"/>
-      <c r="E45" s="22"/>
-      <c r="F45" s="65"/>
-      <c r="G45" s="12"/>
-    </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B46" s="22"/>
-      <c r="C46" s="22"/>
-      <c r="D46" s="22"/>
-      <c r="E46" s="22"/>
-      <c r="F46" s="65"/>
-      <c r="G46" s="12"/>
-    </row>
-    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B47" s="22"/>
-      <c r="C47" s="22"/>
-      <c r="D47" s="22"/>
-      <c r="E47" s="22"/>
-      <c r="F47" s="65"/>
-      <c r="G47" s="12"/>
+      <c r="D47" s="104" t="s">
+        <v>133</v>
+      </c>
+      <c r="E47" s="104" t="s">
+        <v>62</v>
+      </c>
+      <c r="F47" s="105" t="s">
+        <v>134</v>
+      </c>
+      <c r="G47" s="30"/>
+    </row>
+    <row r="48" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B48" s="94"/>
+      <c r="C48" s="104" t="s">
+        <v>135</v>
+      </c>
+      <c r="D48" s="104" t="s">
+        <v>25</v>
+      </c>
+      <c r="E48" s="104" t="s">
+        <v>60</v>
+      </c>
+      <c r="F48" s="105" t="s">
+        <v>136</v>
+      </c>
+      <c r="G48" s="30"/>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B49" s="22"/>
+      <c r="C49" s="22"/>
+      <c r="D49" s="22"/>
+      <c r="E49" s="22"/>
+      <c r="F49" s="65"/>
+      <c r="G49" s="12"/>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B50" s="22"/>
+      <c r="C50" s="22"/>
+      <c r="D50" s="22"/>
+      <c r="E50" s="22"/>
+      <c r="F50" s="65"/>
+      <c r="G50" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="B39:B42"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="B35:B36"/>
+  <mergeCells count="18">
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="B40:B44"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="B29:B32"/>
+    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B9:B13"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="B14:B18"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="B36:B37"/>
     <mergeCell ref="B5:B8"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="B28:B31"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="B25:B27"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="B13:B17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
update exception messages, add list definition
updated exception messages to make debugging easier
added list definition with '[' and ']' commands
reworked List and WordSet recording
</commit_message>
<xml_diff>
--- a/WordList.xlsx
+++ b/WordList.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="173">
   <si>
     <t>Name</t>
   </si>
@@ -528,6 +528,21 @@
   </si>
   <si>
     <t>Sets the object at a given index.</t>
+  </si>
+  <si>
+    <t>[</t>
+  </si>
+  <si>
+    <t>StartList</t>
+  </si>
+  <si>
+    <t>Pushes a StartList object to the stack and starts recording a list.</t>
+  </si>
+  <si>
+    <t>]</t>
+  </si>
+  <si>
+    <t>Ends recording a list and pushes the resulting list to the stack.</t>
   </si>
 </sst>
 </file>
@@ -875,7 +890,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="117">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1075,28 +1090,79 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1105,12 +1171,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1122,48 +1182,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1454,7 +1472,7 @@
   <dimension ref="B1:K70"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I45" sqref="I45"/>
+      <selection activeCell="I54" sqref="I54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1499,10 +1517,10 @@
       <c r="E5" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="104" t="s">
+      <c r="F5" s="87" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="105"/>
+      <c r="G5" s="88"/>
       <c r="J5" s="40" t="s">
         <v>93</v>
       </c>
@@ -1511,7 +1529,7 @@
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="87" t="s">
+      <c r="B6" s="110" t="s">
         <v>85</v>
       </c>
       <c r="C6" s="55" t="s">
@@ -1535,7 +1553,7 @@
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="88"/>
+      <c r="B7" s="99"/>
       <c r="C7" s="11" t="s">
         <v>8</v>
       </c>
@@ -1553,7 +1571,7 @@
       <c r="K7" s="12"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="88"/>
+      <c r="B8" s="99"/>
       <c r="C8" s="11" t="s">
         <v>9</v>
       </c>
@@ -1575,7 +1593,7 @@
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="89"/>
+      <c r="B9" s="100"/>
       <c r="C9" s="11" t="s">
         <v>104</v>
       </c>
@@ -1593,7 +1611,7 @@
       <c r="K9" s="12"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="93" t="s">
+      <c r="B10" s="91" t="s">
         <v>21</v>
       </c>
       <c r="C10" s="27" t="s">
@@ -1615,7 +1633,7 @@
       <c r="K10" s="12"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="107"/>
+      <c r="B11" s="92"/>
       <c r="C11" s="27" t="s">
         <v>139</v>
       </c>
@@ -1633,7 +1651,7 @@
       <c r="K11" s="12"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="107"/>
+      <c r="B12" s="92"/>
       <c r="C12" s="27" t="s">
         <v>5</v>
       </c>
@@ -1655,7 +1673,7 @@
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="107"/>
+      <c r="B13" s="92"/>
       <c r="C13" s="27" t="s">
         <v>6</v>
       </c>
@@ -1673,7 +1691,7 @@
       <c r="K13" s="12"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="94"/>
+      <c r="B14" s="93"/>
       <c r="C14" s="27" t="s">
         <v>37</v>
       </c>
@@ -1691,7 +1709,7 @@
       <c r="K14" s="12"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="90" t="s">
+      <c r="B15" s="103" t="s">
         <v>20</v>
       </c>
       <c r="C15" s="16" t="s">
@@ -1713,7 +1731,7 @@
       <c r="K15" s="12"/>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="91"/>
+      <c r="B16" s="104"/>
       <c r="C16" s="16" t="s">
         <v>10</v>
       </c>
@@ -1733,7 +1751,7 @@
       <c r="K16" s="12"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="91"/>
+      <c r="B17" s="104"/>
       <c r="C17" s="16" t="s">
         <v>145</v>
       </c>
@@ -1753,7 +1771,7 @@
       <c r="K17" s="12"/>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="91"/>
+      <c r="B18" s="104"/>
       <c r="C18" s="16" t="s">
         <v>146</v>
       </c>
@@ -1773,7 +1791,7 @@
       <c r="K18" s="12"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="91"/>
+      <c r="B19" s="104"/>
       <c r="C19" s="16" t="s">
         <v>18</v>
       </c>
@@ -1793,7 +1811,7 @@
       <c r="K19" s="12"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="97" t="s">
+      <c r="B20" s="89" t="s">
         <v>33</v>
       </c>
       <c r="C20" s="45" t="s">
@@ -1813,7 +1831,7 @@
       <c r="K20" s="12"/>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B21" s="106"/>
+      <c r="B21" s="90"/>
       <c r="C21" s="45" t="s">
         <v>86</v>
       </c>
@@ -1831,7 +1849,7 @@
       <c r="K21" s="12"/>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="98"/>
+      <c r="B22" s="108"/>
       <c r="C22" s="46" t="s">
         <v>160</v>
       </c>
@@ -1849,7 +1867,7 @@
       <c r="K22" s="12"/>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="114" t="s">
+      <c r="B23" s="105" t="s">
         <v>44</v>
       </c>
       <c r="C23" s="32" t="s">
@@ -1869,7 +1887,7 @@
       <c r="K23" s="12"/>
     </row>
     <row r="24" spans="2:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="115"/>
+      <c r="B24" s="106"/>
       <c r="C24" s="34" t="s">
         <v>39</v>
       </c>
@@ -1879,15 +1897,15 @@
       <c r="E24" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="F24" s="108" t="s">
+      <c r="F24" s="94" t="s">
         <v>43</v>
       </c>
-      <c r="G24" s="109"/>
+      <c r="G24" s="95"/>
       <c r="J24" s="22"/>
       <c r="K24" s="12"/>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B25" s="116"/>
+      <c r="B25" s="107"/>
       <c r="C25" s="34" t="s">
         <v>123</v>
       </c>
@@ -1905,7 +1923,7 @@
       <c r="K25" s="12"/>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B26" s="110" t="s">
+      <c r="B26" s="96" t="s">
         <v>49</v>
       </c>
       <c r="C26" s="10" t="s">
@@ -1925,7 +1943,7 @@
       <c r="K26" s="12"/>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B27" s="111"/>
+      <c r="B27" s="97"/>
       <c r="C27" s="10" t="s">
         <v>46</v>
       </c>
@@ -1943,7 +1961,7 @@
       <c r="K27" s="12"/>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B28" s="103" t="s">
+      <c r="B28" s="98" t="s">
         <v>55</v>
       </c>
       <c r="C28" s="11" t="s">
@@ -1963,7 +1981,7 @@
       <c r="K28" s="12"/>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B29" s="88"/>
+      <c r="B29" s="99"/>
       <c r="C29" s="11" t="s">
         <v>74</v>
       </c>
@@ -1981,7 +1999,7 @@
       <c r="K29" s="12"/>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B30" s="89"/>
+      <c r="B30" s="100"/>
       <c r="C30" s="38" t="s">
         <v>58</v>
       </c>
@@ -1991,15 +2009,15 @@
       <c r="E30" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="F30" s="112" t="s">
+      <c r="F30" s="101" t="s">
         <v>62</v>
       </c>
-      <c r="G30" s="113"/>
+      <c r="G30" s="102"/>
       <c r="J30" s="22"/>
       <c r="K30" s="12"/>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B31" s="97" t="s">
+      <c r="B31" s="89" t="s">
         <v>72</v>
       </c>
       <c r="C31" s="45" t="s">
@@ -2021,7 +2039,7 @@
       <c r="K31" s="12"/>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B32" s="106"/>
+      <c r="B32" s="90"/>
       <c r="C32" s="45" t="s">
         <v>164</v>
       </c>
@@ -2041,7 +2059,7 @@
       <c r="K32" s="12"/>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B33" s="106"/>
+      <c r="B33" s="90"/>
       <c r="C33" s="45" t="s">
         <v>162</v>
       </c>
@@ -2061,7 +2079,7 @@
       <c r="K33" s="12"/>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B34" s="106"/>
+      <c r="B34" s="90"/>
       <c r="C34" s="45" t="s">
         <v>163</v>
       </c>
@@ -2081,7 +2099,7 @@
       <c r="K34" s="12"/>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B35" s="93" t="s">
+      <c r="B35" s="91" t="s">
         <v>73</v>
       </c>
       <c r="C35" s="23" t="s">
@@ -2103,7 +2121,7 @@
       <c r="K35" s="12"/>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B36" s="107"/>
+      <c r="B36" s="92"/>
       <c r="C36" s="27" t="s">
         <v>75</v>
       </c>
@@ -2123,7 +2141,7 @@
       <c r="K36" s="12"/>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B37" s="94"/>
+      <c r="B37" s="93"/>
       <c r="C37" s="27" t="s">
         <v>76</v>
       </c>
@@ -2143,7 +2161,7 @@
       <c r="K37" s="12"/>
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B38" s="86" t="s">
+      <c r="B38" s="109" t="s">
         <v>94</v>
       </c>
       <c r="C38" s="16" t="s">
@@ -2161,7 +2179,7 @@
       <c r="G38" s="51"/>
     </row>
     <row r="39" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="86"/>
+      <c r="B39" s="109"/>
       <c r="C39" s="52" t="s">
         <v>98</v>
       </c>
@@ -2171,10 +2189,10 @@
       <c r="E39" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="F39" s="99" t="s">
+      <c r="F39" s="114" t="s">
         <v>100</v>
       </c>
-      <c r="G39" s="100"/>
+      <c r="G39" s="115"/>
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B40" s="35" t="s">
@@ -2213,7 +2231,7 @@
       <c r="G41" s="69"/>
     </row>
     <row r="42" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B42" s="103" t="s">
+      <c r="B42" s="98" t="s">
         <v>109</v>
       </c>
       <c r="C42" s="37" t="s">
@@ -2231,7 +2249,7 @@
       <c r="G42" s="71"/>
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B43" s="88"/>
+      <c r="B43" s="99"/>
       <c r="C43" s="37" t="s">
         <v>111</v>
       </c>
@@ -2247,7 +2265,7 @@
       <c r="G43" s="71"/>
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B44" s="88"/>
+      <c r="B44" s="99"/>
       <c r="C44" s="37" t="s">
         <v>115</v>
       </c>
@@ -2263,7 +2281,7 @@
       <c r="G44" s="71"/>
     </row>
     <row r="45" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B45" s="88"/>
+      <c r="B45" s="99"/>
       <c r="C45" s="37" t="s">
         <v>117</v>
       </c>
@@ -2279,7 +2297,7 @@
       <c r="G45" s="71"/>
     </row>
     <row r="46" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B46" s="88"/>
+      <c r="B46" s="99"/>
       <c r="C46" s="37" t="s">
         <v>135</v>
       </c>
@@ -2295,7 +2313,7 @@
       <c r="G46" s="71"/>
     </row>
     <row r="47" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="89"/>
+      <c r="B47" s="100"/>
       <c r="C47" s="37" t="s">
         <v>157</v>
       </c>
@@ -2305,13 +2323,13 @@
       <c r="E47" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="F47" s="101" t="s">
+      <c r="F47" s="116" t="s">
         <v>159</v>
       </c>
-      <c r="G47" s="102"/>
+      <c r="G47" s="117"/>
     </row>
     <row r="48" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B48" s="97" t="s">
+      <c r="B48" s="89" t="s">
         <v>119</v>
       </c>
       <c r="C48" s="72" t="s">
@@ -2329,7 +2347,7 @@
       <c r="G48" s="74"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B49" s="98"/>
+      <c r="B49" s="108"/>
       <c r="C49" s="72" t="s">
         <v>131</v>
       </c>
@@ -2339,13 +2357,13 @@
       <c r="E49" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="F49" s="95" t="s">
+      <c r="F49" s="112" t="s">
         <v>134</v>
       </c>
-      <c r="G49" s="96"/>
+      <c r="G49" s="113"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B50" s="93" t="s">
+      <c r="B50" s="91" t="s">
         <v>125</v>
       </c>
       <c r="C50" s="78" t="s">
@@ -2363,7 +2381,7 @@
       <c r="G50" s="30"/>
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B51" s="94"/>
+      <c r="B51" s="93"/>
       <c r="C51" s="78" t="s">
         <v>129</v>
       </c>
@@ -2379,7 +2397,7 @@
       <c r="G51" s="30"/>
     </row>
     <row r="52" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B52" s="90" t="s">
+      <c r="B52" s="103" t="s">
         <v>141</v>
       </c>
       <c r="C52" s="77" t="s">
@@ -2397,7 +2415,7 @@
       <c r="G52" s="51"/>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B53" s="91"/>
+      <c r="B53" s="104"/>
       <c r="C53" s="77" t="s">
         <v>150</v>
       </c>
@@ -2413,7 +2431,7 @@
       <c r="G53" s="51"/>
     </row>
     <row r="54" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B54" s="91"/>
+      <c r="B54" s="104"/>
       <c r="C54" s="77" t="s">
         <v>17</v>
       </c>
@@ -2429,7 +2447,7 @@
       <c r="G54" s="83"/>
     </row>
     <row r="55" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B55" s="91"/>
+      <c r="B55" s="104"/>
       <c r="C55" s="77" t="s">
         <v>152</v>
       </c>
@@ -2445,7 +2463,7 @@
       <c r="G55" s="83"/>
     </row>
     <row r="56" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B56" s="91"/>
+      <c r="B56" s="104"/>
       <c r="C56" s="85" t="s">
         <v>165</v>
       </c>
@@ -2461,7 +2479,7 @@
       <c r="G56" s="83"/>
     </row>
     <row r="57" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B57" s="92"/>
+      <c r="B57" s="104"/>
       <c r="C57" s="77" t="s">
         <v>155</v>
       </c>
@@ -2477,20 +2495,36 @@
       <c r="G57" s="83"/>
     </row>
     <row r="58" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B58" s="22"/>
-      <c r="C58" s="22"/>
-      <c r="D58" s="22"/>
-      <c r="E58" s="22"/>
-      <c r="F58" s="81"/>
-      <c r="G58" s="80"/>
+      <c r="B58" s="104"/>
+      <c r="C58" s="86" t="s">
+        <v>168</v>
+      </c>
+      <c r="D58" s="86" t="s">
+        <v>10</v>
+      </c>
+      <c r="E58" s="86" t="s">
+        <v>169</v>
+      </c>
+      <c r="F58" s="84" t="s">
+        <v>170</v>
+      </c>
+      <c r="G58" s="83"/>
     </row>
     <row r="59" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B59" s="22"/>
-      <c r="C59" s="22"/>
-      <c r="D59" s="22"/>
-      <c r="E59" s="22"/>
-      <c r="F59" s="81"/>
-      <c r="G59" s="80"/>
+      <c r="B59" s="111"/>
+      <c r="C59" s="86" t="s">
+        <v>171</v>
+      </c>
+      <c r="D59" s="86" t="s">
+        <v>54</v>
+      </c>
+      <c r="E59" s="86" t="s">
+        <v>141</v>
+      </c>
+      <c r="F59" s="84" t="s">
+        <v>172</v>
+      </c>
+      <c r="G59" s="83"/>
     </row>
     <row r="60" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B60" s="22"/>
@@ -2582,6 +2616,15 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="B42:B47"/>
+    <mergeCell ref="B52:B59"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="B31:B34"/>
     <mergeCell ref="B35:B37"/>
@@ -2593,15 +2636,6 @@
     <mergeCell ref="B15:B19"/>
     <mergeCell ref="B23:B25"/>
     <mergeCell ref="B20:B22"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="B52:B57"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="F49:G49"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="F47:G47"/>
-    <mergeCell ref="B42:B47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>